<commit_message>
changed MPS field in revenue report
</commit_message>
<xml_diff>
--- a/src/main/resources/revenueReportTemplate.xlsx
+++ b/src/main/resources/revenueReportTemplate.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="348" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="348" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Отчет" sheetId="2" r:id="rId1"/>
     <sheet name="Rejects, Сhargebacks" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="19">
   <si>
     <t>Gross (Брутто)</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>Причина</t>
+  </si>
+  <si>
+    <t>МПС</t>
   </si>
 </sst>
 </file>
@@ -527,11 +530,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -842,29 +845,31 @@
   <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" style="7" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" style="7" customWidth="1"/>
-    <col min="5" max="8" width="11.42578125" style="7" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" style="7" customWidth="1"/>
-    <col min="10" max="11" width="11.7109375" style="7" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" style="7" customWidth="1"/>
+    <col min="5" max="8" width="11.44140625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="10.109375" style="7" customWidth="1"/>
+    <col min="10" max="11" width="11.6640625" style="7" customWidth="1"/>
+    <col min="12" max="12" width="11.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" style="7" customWidth="1"/>
     <col min="14" max="14" width="9" style="7" customWidth="1"/>
-    <col min="15" max="15" width="16.42578125" style="7" customWidth="1"/>
+    <col min="15" max="15" width="16.44140625" style="7" customWidth="1"/>
     <col min="16" max="17" width="12" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.42578125" style="7" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="7"/>
+    <col min="18" max="18" width="10.44140625" style="7" customWidth="1"/>
+    <col min="19" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11"/>
+    <row r="1" spans="1:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>18</v>
+      </c>
       <c r="B1" s="15" t="s">
         <v>3</v>
       </c>
@@ -902,7 +907,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12"/>
       <c r="B2" s="16"/>
       <c r="C2" s="23"/>
@@ -952,7 +957,7 @@
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
     </row>
-    <row r="4" spans="1:19" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="19" t="s">
         <v>14</v>
       </c>
@@ -1023,29 +1028,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" style="7" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" style="7" customWidth="1"/>
-    <col min="5" max="8" width="11.42578125" style="7" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" style="7" customWidth="1"/>
-    <col min="10" max="11" width="11.7109375" style="7" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" style="7" customWidth="1"/>
+    <col min="5" max="8" width="11.44140625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="10.109375" style="7" customWidth="1"/>
+    <col min="10" max="11" width="11.6640625" style="7" customWidth="1"/>
+    <col min="12" max="12" width="11.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" style="7" customWidth="1"/>
     <col min="14" max="14" width="9" style="7" customWidth="1"/>
-    <col min="15" max="15" width="16.42578125" style="7" customWidth="1"/>
+    <col min="15" max="15" width="16.44140625" style="7" customWidth="1"/>
     <col min="16" max="17" width="12" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.42578125" style="7" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="7"/>
+    <col min="18" max="18" width="10.44140625" style="7" customWidth="1"/>
+    <col min="19" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11"/>
       <c r="B1" s="15" t="s">
         <v>3</v>
@@ -1080,14 +1085,14 @@
       <c r="P1" s="26"/>
       <c r="Q1" s="26"/>
       <c r="R1" s="28"/>
-      <c r="S1" s="32" t="s">
+      <c r="S1" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="T1" s="33" t="s">
+      <c r="T1" s="32" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12"/>
       <c r="B2" s="16"/>
       <c r="C2" s="23"/>
@@ -1138,7 +1143,7 @@
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
     </row>
-    <row r="4" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="19" t="s">
         <v>14</v>
       </c>
@@ -1188,6 +1193,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:S4"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="T1:T2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:I1"/>
@@ -1195,11 +1205,6 @@
     <mergeCell ref="J1:N1"/>
     <mergeCell ref="O1:R1"/>
     <mergeCell ref="S1:S2"/>
-    <mergeCell ref="A4:S4"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>